<commit_message>
Updating the reference guide
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354AB37D-C461-47E5-97BE-214C10CC0E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860DDECB-029A-46AE-AC46-028B19094F45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Description</t>
   </si>
@@ -149,9 +149,6 @@
 Ground Stomp: 1d8 damage to 2 enemies</t>
   </si>
   <si>
-    <t>ElementalWeaknesses</t>
-  </si>
-  <si>
     <t>Water</t>
   </si>
   <si>
@@ -163,6 +160,44 @@
   </si>
   <si>
     <t>Spend 1 SP to summon a Wolf to your side if in a forest.  Wolf has 4 HP and can do 1d6 damage and has its own turn during combat.</t>
+  </si>
+  <si>
+    <t>Muskroom</t>
+  </si>
+  <si>
+    <t>A muskrat covered in mushrooms</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Scratch: 1d4+3 damage
+Bite: 1d4 damage.  Causes Poison.
+Spore Cloud: Cause Poison on all enemies</t>
+  </si>
+  <si>
+    <t>Weakness</t>
+  </si>
+  <si>
+    <t>Flying Drone</t>
+  </si>
+  <si>
+    <t>A robot in the air that can shoot an enemy</t>
+  </si>
+  <si>
+    <t>Lightning</t>
+  </si>
+  <si>
+    <t>Laser Shot: 1d6 damage</t>
+  </si>
+  <si>
+    <t>Dangerous Mushroom</t>
+  </si>
+  <si>
+    <t>Requires a resilience roll:
+-	Success: Heal 1d6 HP
+-	Minor Success: Heal 1d6 HP but gain Poison.
+-	Fail: Gain Poison</t>
   </si>
 </sst>
 </file>
@@ -280,7 +315,7 @@
     <tableColumn id="2" xr3:uid="{85408EF0-217C-4099-B9B4-76C10B3F0E78}" name="Description" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{A5EC2A9A-6BA1-4B7D-B5DA-8C9224EA5B81}" name="HP" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{924C6403-8AE8-4669-A217-B9ABBEF740DB}" name="Armor" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{6CC9B910-033B-40F4-969A-97A391A050CF}" name="ElementalWeaknesses" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{6CC9B910-033B-40F4-969A-97A391A050CF}" name="Weakness" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{6B8EAA1A-2A00-4C9B-A08B-44BB1FEECCFA}" name="Attacks" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -288,11 +323,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D599C6E-A039-49D0-9665-149D27B2EC46}" name="Table3" displayName="Table3" ref="A1:B20" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D599C6E-A039-49D0-9665-149D27B2EC46}" name="Table3" displayName="Table3" ref="A1:B20" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="A1:B20" xr:uid="{6A194999-3725-461E-838F-D2C813311D1A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3FF4632E-6B09-412C-A4A3-C80FF13A2A4D}" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{8D016556-DD86-46D2-B06B-066E93A5DEA6}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3FF4632E-6B09-412C-A4A3-C80FF13A2A4D}" name="Name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{8D016556-DD86-46D2-B06B-066E93A5DEA6}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -595,15 +630,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD07E7A-4503-4B4C-9531-FC2C793E7E47}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
   </cols>
@@ -749,6 +784,17 @@
       </c>
       <c r="C13">
         <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -764,7 +810,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,7 +836,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -810,7 +856,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>28</v>
@@ -830,27 +876,51 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1049,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2F0500-CC62-4BD5-9B1C-FA93D6A66B6C}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1069,10 +1139,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Trying to fix name generator
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860DDECB-029A-46AE-AC46-028B19094F45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA6688B-11FF-4492-A8B0-8126F1CA693C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
     <sheet name="Bestiary" sheetId="2" r:id="rId2"/>
-    <sheet name="SampleCustomMoves" sheetId="3" r:id="rId3"/>
+    <sheet name="Sample_Custom_Moves" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
   <si>
     <t>Description</t>
   </si>
@@ -127,9 +127,6 @@
 Dirt Tail Whip: 1d6 ranged Earth damage plus causes Blind.</t>
   </si>
   <si>
-    <t>Tonic</t>
-  </si>
-  <si>
     <t>Tincture</t>
   </si>
   <si>
@@ -150,10 +147,6 @@
   </si>
   <si>
     <t>Water</t>
-  </si>
-  <si>
-    <t>Fire
-Lightning</t>
   </si>
   <si>
     <t>Call of the Wild</t>
@@ -198,6 +191,52 @@
 -	Success: Heal 1d6 HP
 -	Minor Success: Heal 1d6 HP but gain Poison.
 -	Fail: Gain Poison</t>
+  </si>
+  <si>
+    <t>Potion+</t>
+  </si>
+  <si>
+    <t>Heals All HP</t>
+  </si>
+  <si>
+    <t>Tincture+</t>
+  </si>
+  <si>
+    <t>Heals all HP and SP</t>
+  </si>
+  <si>
+    <t>Concoction+</t>
+  </si>
+  <si>
+    <t>Heals all SP</t>
+  </si>
+  <si>
+    <t>Brew</t>
+  </si>
+  <si>
+    <t>Lazarus Tonic</t>
+  </si>
+  <si>
+    <t>Revives a fainted comrade in battle</t>
+  </si>
+  <si>
+    <t>Gunner Soldier</t>
+  </si>
+  <si>
+    <t>A soldier with a gun</t>
+  </si>
+  <si>
+    <t>Gunshot: 1d10 damage to an enemy
+Gun Spray: 1d4 damage to all enemies</t>
+  </si>
+  <si>
+    <t>Prosecutor</t>
+  </si>
+  <si>
+    <t>+1 to Diplomacy when you try to convince others that someone is lying (whether it's true or not)</t>
+  </si>
+  <si>
+    <t>Fire, Lightning</t>
   </si>
 </sst>
 </file>
@@ -233,12 +272,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -630,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD07E7A-4503-4B4C-9531-FC2C793E7E47}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +753,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -777,10 +819,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
         <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
       </c>
       <c r="C13">
         <v>30</v>
@@ -788,13 +830,57 @@
     </row>
     <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14">
         <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -810,7 +896,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +922,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -847,7 +933,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1">
         <v>10</v>
@@ -856,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>28</v>
@@ -864,10 +950,10 @@
     </row>
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C3" s="1">
         <v>10</v>
@@ -876,18 +962,18 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -896,18 +982,18 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
@@ -916,19 +1002,29 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="1">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -1120,7 +1216,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,15 +1235,19 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>

</xml_diff>

<commit_message>
Adding multiple creatures to bestiary
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\TerraMachina\site\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07786AC1-FDA9-46CB-937A-7FFD80949C01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B62007-F855-476D-BF97-5DE5CA38E9BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Description</t>
   </si>
@@ -242,6 +242,62 @@
   </si>
   <si>
     <t>+1 to Engineering for creating a delicious meal that will restore 1d4 HP or SP</t>
+  </si>
+  <si>
+    <t>Fire Scorpion</t>
+  </si>
+  <si>
+    <t>A big scorpion that has does fire damage</t>
+  </si>
+  <si>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>Sting: 1d12 fire damage.  Causes burn.
+Pinch: 1d4.  Traps the player who must make a move to escape.</t>
+  </si>
+  <si>
+    <t>Crystal Squid</t>
+  </si>
+  <si>
+    <t>A squid that can swim</t>
+  </si>
+  <si>
+    <t>Snap: 1d10 damage to a single player
+Embrace: 1d4 damage.  Traps the player who must make a move to escape
+Water Jet: 1d10 damage to all players</t>
+  </si>
+  <si>
+    <t>Magmus</t>
+  </si>
+  <si>
+    <t>A humanoid creature made of lava rock</t>
+  </si>
+  <si>
+    <t>Fire Punch: 1d8 Fire damage.</t>
+  </si>
+  <si>
+    <t>Baterina</t>
+  </si>
+  <si>
+    <t>A giant back with legs that wears a tutu</t>
+  </si>
+  <si>
+    <t>Holy</t>
+  </si>
+  <si>
+    <t>Bite: 1d12 damage.  Causes Mania</t>
+  </si>
+  <si>
+    <t>Snow Vixen</t>
+  </si>
+  <si>
+    <t>Bite: 1d10 damage
+Scratch: 1d6 damage
+Snow Beam: 1d10 Ice damage</t>
+  </si>
+  <si>
+    <t>A giant white fox</t>
   </si>
 </sst>
 </file>
@@ -900,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191A2584-3C3A-4478-9F02-7F1AAD4EB254}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,45 +1087,105 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="1">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="1">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="1">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="1">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1220,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2F0500-CC62-4BD5-9B1C-FA93D6A66B6C}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updating documents + adding ability to delete npcs
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B62007-F855-476D-BF97-5DE5CA38E9BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B86AD7-7211-4697-8E5F-7DF45BFE7A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
   <si>
     <t>Description</t>
   </si>
@@ -145,9 +145,6 @@
 Ground Stomp: 1d8 damage to 2 enemies</t>
   </si>
   <si>
-    <t>Water</t>
-  </si>
-  <si>
     <t>Call of the Wild</t>
   </si>
   <si>
@@ -186,12 +183,6 @@
     <t>Dangerous Mushroom</t>
   </si>
   <si>
-    <t>Requires a resilience roll:
--	Success: Heal 1d6 HP
--	Minor Success: Heal 1d6 HP but gain Poison.
--	Fail: Gain Poison</t>
-  </si>
-  <si>
     <t>Potion+</t>
   </si>
   <si>
@@ -239,9 +230,6 @@
   </si>
   <si>
     <t>Chef</t>
-  </si>
-  <si>
-    <t>+1 to Engineering for creating a delicious meal that will restore 1d4 HP or SP</t>
   </si>
   <si>
     <t>Fire Scorpion</t>
@@ -298,6 +286,82 @@
   </si>
   <si>
     <t>A giant white fox</t>
+  </si>
+  <si>
+    <t>+1 to Tinker for creating a delicious meal that will restore 1d4 HP or SP</t>
+  </si>
+  <si>
+    <t>Informed Traveller</t>
+  </si>
+  <si>
+    <t>+1 to Knowledge roll for a city/town you haven't been to before</t>
+  </si>
+  <si>
+    <t>Dark Wolf</t>
+  </si>
+  <si>
+    <t>A tall wolf with charcoal-like skin</t>
+  </si>
+  <si>
+    <t>Bite: 1d10 damage</t>
+  </si>
+  <si>
+    <t>Welder's Gloves</t>
+  </si>
+  <si>
+    <t>Gloves that add +1 to Tinker</t>
+  </si>
+  <si>
+    <t>Rock Beast</t>
+  </si>
+  <si>
+    <t>A humanoid creature made of dirt and rock</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Rock Punch: 1d10 Earth damage
+Grab: Entrap an enemy</t>
+  </si>
+  <si>
+    <t>Ring of Fire</t>
+  </si>
+  <si>
+    <t>A literal floating circle of fire</t>
+  </si>
+  <si>
+    <t>Marionette</t>
+  </si>
+  <si>
+    <t>A marionette.  A puppet on strings.</t>
+  </si>
+  <si>
+    <t>Fireball: 1d8 fire damage.  Causes Burn.</t>
+  </si>
+  <si>
+    <t>Slap: 1d8 damage</t>
+  </si>
+  <si>
+    <t>Iridescent Scale</t>
+  </si>
+  <si>
+    <t>Material that can be used for making things.  Adds a glow.</t>
+  </si>
+  <si>
+    <t>Requires a resilience roll:
+-	Success: Heal 1d6 HP
+-	Minor Success: Heal 1d6 HP but gain Poison
+-	Fail: Gain Poison</t>
+  </si>
+  <si>
+    <t>Skeleton Knight</t>
+  </si>
+  <si>
+    <t>A skeleton in armor with a sword</t>
+  </si>
+  <si>
+    <t>Slash: 1d8 damage</t>
   </si>
 </sst>
 </file>
@@ -733,16 +797,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD07E7A-4503-4B4C-9531-FC2C793E7E47}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -814,7 +878,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -891,10 +955,10 @@
     </row>
     <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -902,10 +966,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15">
         <v>25</v>
@@ -913,10 +977,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16">
         <v>70</v>
@@ -924,10 +988,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>25</v>
@@ -935,13 +999,35 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -956,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191A2584-3C3A-4478-9F02-7F1AAD4EB254}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +1069,7 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>10</v>
@@ -1003,7 +1089,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>28</v>
@@ -1023,7 +1109,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>34</v>
@@ -1031,10 +1117,10 @@
     </row>
     <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -1043,18 +1129,18 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
@@ -1063,18 +1149,18 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1">
         <v>7</v>
@@ -1084,15 +1170,15 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C7" s="1">
         <v>14</v>
@@ -1101,18 +1187,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C8" s="1">
         <v>13</v>
@@ -1121,18 +1207,18 @@
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
@@ -1141,18 +1227,18 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1">
         <v>6</v>
@@ -1161,18 +1247,18 @@
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C11" s="1">
         <v>11</v>
@@ -1181,51 +1267,111 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="1">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="1">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1337,7 +1483,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,31 +1502,35 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>

</xml_diff>

<commit_message>
Terra Machina Reference Guide
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B86AD7-7211-4697-8E5F-7DF45BFE7A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3159ABBC-EA3E-4357-918C-9F9B43064294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="132">
   <si>
     <t>Description</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Informed Traveller</t>
   </si>
   <si>
-    <t>+1 to Knowledge roll for a city/town you haven't been to before</t>
-  </si>
-  <si>
     <t>Dark Wolf</t>
   </si>
   <si>
@@ -341,12 +338,6 @@
   </si>
   <si>
     <t>Slap: 1d8 damage</t>
-  </si>
-  <si>
-    <t>Iridescent Scale</t>
-  </si>
-  <si>
-    <t>Material that can be used for making things.  Adds a glow.</t>
   </si>
   <si>
     <t>Requires a resilience roll:
@@ -362,6 +353,99 @@
   </si>
   <si>
     <t>Slash: 1d8 damage</t>
+  </si>
+  <si>
+    <t>Ring of Lightning</t>
+  </si>
+  <si>
+    <t>A literal floating circle of electricity</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Lightning Strike: 1d8 Lightning damage.  Causes Paralysis.</t>
+  </si>
+  <si>
+    <t>+1 to Knowledge roll for information about a city/town you haven't been to before</t>
+  </si>
+  <si>
+    <t>Cavern Explorer</t>
+  </si>
+  <si>
+    <t>+1 to Sense roll when inside a cave or cavern</t>
+  </si>
+  <si>
+    <t>+1 to next Diplomacy Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Movement Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Shoot Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Deduction Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Knowledge Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Tinker Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Brawn Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Melee Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Resilience Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Energy Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Search Roll</t>
+  </si>
+  <si>
+    <t>+1 to next Sense Roll</t>
+  </si>
+  <si>
+    <t>Confidence Booster</t>
+  </si>
+  <si>
+    <t>Brain Boost</t>
+  </si>
+  <si>
+    <t>Encyclopedia Light</t>
+  </si>
+  <si>
+    <t>Steroid</t>
+  </si>
+  <si>
+    <t>Vitamin</t>
+  </si>
+  <si>
+    <t>Magnifier</t>
+  </si>
+  <si>
+    <t>Concentration</t>
+  </si>
+  <si>
+    <t>Elbow Grease</t>
+  </si>
+  <si>
+    <t>Brawl Balm</t>
+  </si>
+  <si>
+    <t>Flex</t>
+  </si>
+  <si>
+    <t>Energy Boost</t>
+  </si>
+  <si>
+    <t>Enhancer</t>
   </si>
 </sst>
 </file>
@@ -397,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -408,6 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,8 +545,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFB740B0-BE3C-48D7-8B7D-8A37A68A10EB}" name="Table1" displayName="Table1" ref="A1:C26" totalsRowShown="0">
-  <autoFilter ref="A1:C26" xr:uid="{C8901F27-5F41-43F5-95FC-AD34D4A230AC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFB740B0-BE3C-48D7-8B7D-8A37A68A10EB}" name="Table1" displayName="Table1" ref="A1:C31" totalsRowShown="0">
+  <autoFilter ref="A1:C31" xr:uid="{C8901F27-5F41-43F5-95FC-AD34D4A230AC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C11">
     <sortCondition ref="A1:A26"/>
   </sortState>
@@ -477,6 +562,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BF78CB2E-8945-46AD-ADE2-A57C11F5C733}" name="Table2" displayName="Table2" ref="A1:F28" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:F28" xr:uid="{D4A8C1E5-52B8-4BF4-8E93-B0DC341A2D32}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
+    <sortCondition ref="A1:A28"/>
+  </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B84A019F-5E00-493A-A26D-FB72EA88248D}" name="Name" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{85408EF0-217C-4099-B9B4-76C10B3F0E78}" name="Description" dataDxfId="7"/>
@@ -797,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD07E7A-4503-4B4C-9531-FC2C793E7E47}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +1046,7 @@
         <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -1010,10 +1098,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" t="s">
         <v>86</v>
-      </c>
-      <c r="B19" t="s">
-        <v>87</v>
       </c>
       <c r="C19">
         <v>22</v>
@@ -1021,19 +1109,141 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" t="s">
-        <v>99</v>
+        <v>120</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1042,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191A2584-3C3A-4478-9F02-7F1AAD4EB254}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,75 +1285,75 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1">
         <v>10</v>
       </c>
       <c r="D2" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="1">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1152,25 +1362,27 @@
         <v>44</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1193,15 +1405,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1210,58 +1422,56 @@
         <v>44</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C10" s="1">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="1">
         <v>6</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="1">
-        <v>11</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -1270,116 +1480,128 @@
         <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C14" s="1">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="1">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" s="1">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C15" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="1">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="F16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="1">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1">
-        <v>4</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="C17" s="1">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -1483,7 +1705,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,12 +1751,16 @@
         <v>81</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
Updating name generator and documents
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3159ABBC-EA3E-4357-918C-9F9B43064294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C89598-7935-4AE0-A3F6-B8AA9A3EDB51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="139">
   <si>
     <t>Description</t>
   </si>
@@ -446,6 +446,29 @@
   </si>
   <si>
     <t>Enhancer</t>
+  </si>
+  <si>
+    <t>Waterbone</t>
+  </si>
+  <si>
+    <t>A skeleton inside a bubble of water</t>
+  </si>
+  <si>
+    <t>Holy, Lightning</t>
+  </si>
+  <si>
+    <t>Bubble Attack: 1d10 Water damage
+Bone Attack: 1d12 Dark damage.</t>
+  </si>
+  <si>
+    <t>Electric Eel</t>
+  </si>
+  <si>
+    <t>An underwater creature that shoots electricity</t>
+  </si>
+  <si>
+    <t>Bite: 1d10 damage
+Shock: 1d8 Lightning damage to all enemies.  Causes Paralysis.</t>
   </si>
 </sst>
 </file>
@@ -887,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD07E7A-4503-4B4C-9531-FC2C793E7E47}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191A2584-3C3A-4478-9F02-7F1AAD4EB254}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,21 +1626,43 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="1">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="1">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1705,7 +1750,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding to bestiary and starting trap generator
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C89598-7935-4AE0-A3F6-B8AA9A3EDB51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D8BB59-AED7-4CB8-B95C-677F31886CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="142">
   <si>
     <t>Description</t>
   </si>
@@ -469,6 +469,15 @@
   <si>
     <t>Bite: 1d10 damage
 Shock: 1d8 Lightning damage to all enemies.  Causes Paralysis.</t>
+  </si>
+  <si>
+    <t>Giant Weasel</t>
+  </si>
+  <si>
+    <t>A giant weasel</t>
+  </si>
+  <si>
+    <t>Attack: 1d6 damage</t>
   </si>
 </sst>
 </file>
@@ -1275,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191A2584-3C3A-4478-9F02-7F1AAD4EB254}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,267 +1419,277 @@
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>14</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>7</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>10</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="1">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1">
-        <v>4</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C12" s="1">
         <v>7</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D12" s="1">
         <v>2</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C15" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C16" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C17" s="1">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="C18" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>134</v>
+        <v>75</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>136</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>137</v>
+        <v>79</v>
       </c>
       <c r="C19" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F19" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="1">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>

</xml_diff>

<commit_message>
Adding to reference guide and updating pdf
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D8BB59-AED7-4CB8-B95C-677F31886CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFD3867-B1FB-4D5D-8580-6DC37A133709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="144">
   <si>
     <t>Description</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>Attack: 1d6 damage</t>
+  </si>
+  <si>
+    <t>Mountain Climber</t>
+  </si>
+  <si>
+    <t>+1 to Brawn roll for climbing mountains</t>
   </si>
 </sst>
 </file>
@@ -1284,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191A2584-3C3A-4478-9F02-7F1AAD4EB254}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2F0500-CC62-4BD5-9B1C-FA93D6A66B6C}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,8 +1833,12 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>

</xml_diff>

<commit_message>
multiple changes to ref, randomizers, and site
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFD3867-B1FB-4D5D-8580-6DC37A133709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F0FD0D-C712-418F-8E6E-149DFE6BFAB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="151">
   <si>
     <t>Description</t>
   </si>
@@ -484,6 +484,27 @@
   </si>
   <si>
     <t>+1 to Brawn roll for climbing mountains</t>
+  </si>
+  <si>
+    <t>+1 to Sense roll when listening to others' conversations</t>
+  </si>
+  <si>
+    <t>Big Ears</t>
+  </si>
+  <si>
+    <t>Walking Shark</t>
+  </si>
+  <si>
+    <t>A shark on two legs</t>
+  </si>
+  <si>
+    <t>Bite: 1d10 damage.  Once bitten, 3 damage every turn until the enemy escapes.</t>
+  </si>
+  <si>
+    <t>Detective</t>
+  </si>
+  <si>
+    <t>+1 to Search when investigating a crime</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1312,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,12 +1719,24 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="1">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -1775,7 +1808,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,12 +1874,20 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>

</xml_diff>

<commit_message>
Updating docs + fixing d1 + updates
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79BE7B8-B696-4574-A3C4-D232747953A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E39C09-A33F-4559-B8BE-76DA1A9F32D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>Scale Armor</t>
   </si>
   <si>
-    <t>Adds +1 Armor</t>
-  </si>
-  <si>
     <t>Scratch: 1d8+3 damage
 Bite: 1d8 damage.  Will latch onto a character causing the following: -1 to Movement Rolls and automatic 1d4 damage until free
 Dirt Tail Whip: 1d6 ranged Earth damage plus causes Blind.</t>
@@ -223,9 +220,6 @@
     <t>Prosecutor</t>
   </si>
   <si>
-    <t>+1 to Diplomacy when you try to convince others that someone is lying (whether it's true or not)</t>
-  </si>
-  <si>
     <t>Fire, Lightning</t>
   </si>
   <si>
@@ -288,9 +282,6 @@
     <t>A giant white fox</t>
   </si>
   <si>
-    <t>+1 to Tinker for creating a delicious meal that will restore 1d4 HP or SP</t>
-  </si>
-  <si>
     <t>Informed Traveller</t>
   </si>
   <si>
@@ -304,9 +295,6 @@
   </si>
   <si>
     <t>Welder's Gloves</t>
-  </si>
-  <si>
-    <t>Gloves that add +1 to Tinker</t>
   </si>
   <si>
     <t>Rock Beast</t>
@@ -367,49 +355,7 @@
     <t>Lightning Strike: 1d8 Lightning damage.  Causes Paralysis.</t>
   </si>
   <si>
-    <t>+1 to Knowledge roll for information about a city/town you haven't been to before</t>
-  </si>
-  <si>
     <t>Cavern Explorer</t>
-  </si>
-  <si>
-    <t>+1 to Sense roll when inside a cave or cavern</t>
-  </si>
-  <si>
-    <t>+1 to next Diplomacy Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Movement Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Shoot Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Deduction Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Knowledge Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Tinker Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Brawn Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Melee Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Resilience Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Energy Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Search Roll</t>
-  </si>
-  <si>
-    <t>+1 to next Sense Roll</t>
   </si>
   <si>
     <t>Confidence Booster</t>
@@ -483,12 +429,6 @@
     <t>Mountain Climber</t>
   </si>
   <si>
-    <t>+1 to Brawn roll for climbing mountains</t>
-  </si>
-  <si>
-    <t>+1 to Sense roll when listening to others' conversations</t>
-  </si>
-  <si>
     <t>Big Ears</t>
   </si>
   <si>
@@ -504,9 +444,6 @@
     <t>Detective</t>
   </si>
   <si>
-    <t>+1 to Search when investigating a crime</t>
-  </si>
-  <si>
     <t>Basic Armor</t>
   </si>
   <si>
@@ -571,6 +508,69 @@
   </si>
   <si>
     <t>Plains, Cave, Mountain</t>
+  </si>
+  <si>
+    <t>+2 to Sense roll when listening to others' conversations</t>
+  </si>
+  <si>
+    <t>+2 to Sense roll when inside a cave or cavern</t>
+  </si>
+  <si>
+    <t>+2 to Tinker for creating a delicious meal that will restore 1d4 HP or SP</t>
+  </si>
+  <si>
+    <t>+2 to Search when investigating a crime</t>
+  </si>
+  <si>
+    <t>+2 to Knowledge roll for information about a city/town you haven't been to before</t>
+  </si>
+  <si>
+    <t>+2 to Brawn roll for climbing mountains</t>
+  </si>
+  <si>
+    <t>+2 to Diplomacy when you try to convince others that someone is lying (whether it's true or not)</t>
+  </si>
+  <si>
+    <t>+2 to next Deduction Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Melee Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Shoot Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Diplomacy Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Tinker Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Knowledge Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Energy Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Sense Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Movement Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Search Roll</t>
+  </si>
+  <si>
+    <t>Adds +2 Armor</t>
+  </si>
+  <si>
+    <t>+2 to next Brawn Roll</t>
+  </si>
+  <si>
+    <t>+2 to next Resilience Roll</t>
+  </si>
+  <si>
+    <t>Gloves that add +2 to Tinker</t>
   </si>
 </sst>
 </file>
@@ -624,10 +624,7 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -636,7 +633,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -701,24 +701,24 @@
     <tableColumn id="2" xr3:uid="{85408EF0-217C-4099-B9B4-76C10B3F0E78}" name="Description" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{A5EC2A9A-6BA1-4B7D-B5DA-8C9224EA5B81}" name="HP" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{924C6403-8AE8-4669-A217-B9ABBEF740DB}" name="Armor" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{E94C2E24-8220-4F09-9B67-A8F1D9E335A6}" name="Immunity" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{3104903E-25C1-443A-BC98-4CFAFA3CE060}" name="Locations" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{6CC9B910-033B-40F4-969A-97A391A050CF}" name="Weakness" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{6B8EAA1A-2A00-4C9B-A08B-44BB1FEECCFA}" name="Attacks" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{E94C2E24-8220-4F09-9B67-A8F1D9E335A6}" name="Immunity" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{3104903E-25C1-443A-BC98-4CFAFA3CE060}" name="Locations" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{6CC9B910-033B-40F4-969A-97A391A050CF}" name="Weakness" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{6B8EAA1A-2A00-4C9B-A08B-44BB1FEECCFA}" name="Attacks" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D599C6E-A039-49D0-9665-149D27B2EC46}" name="Table3" displayName="Table3" ref="A1:B20" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7D599C6E-A039-49D0-9665-149D27B2EC46}" name="Table3" displayName="Table3" ref="A1:B20" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="A1:B20" xr:uid="{6A194999-3725-461E-838F-D2C813311D1A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
     <sortCondition ref="A1:A20"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3FF4632E-6B09-412C-A4A3-C80FF13A2A4D}" name="Name" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{8D016556-DD86-46D2-B06B-066E93A5DEA6}" name="Description" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3FF4632E-6B09-412C-A4A3-C80FF13A2A4D}" name="Name" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{8D016556-DD86-46D2-B06B-066E93A5DEA6}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1023,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD07E7A-4503-4B4C-9531-FC2C793E7E47}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,10 +1080,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="C5">
         <v>15</v>
@@ -1091,10 +1091,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -1113,10 +1113,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="C8">
         <v>15</v>
@@ -1135,10 +1135,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>52</v>
       </c>
       <c r="C10">
         <v>25</v>
@@ -1146,10 +1146,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="C11">
         <v>15</v>
@@ -1157,10 +1157,10 @@
     </row>
     <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="C13">
         <v>15</v>
@@ -1179,10 +1179,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>112</v>
+        <v>164</v>
       </c>
       <c r="C14">
         <v>15</v>
@@ -1190,10 +1190,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="C15">
         <v>15</v>
@@ -1201,10 +1201,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="C18">
         <v>15</v>
@@ -1234,10 +1234,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
       </c>
       <c r="C19">
         <v>100</v>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>118</v>
+        <v>168</v>
       </c>
       <c r="C20">
         <v>15</v>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
         <v>47</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
       </c>
       <c r="C25">
         <v>25</v>
@@ -1314,7 +1314,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>169</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -1322,10 +1322,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="C27">
         <v>15</v>
@@ -1333,10 +1333,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
         <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
       </c>
       <c r="C28">
         <v>30</v>
@@ -1344,10 +1344,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" t="s">
         <v>49</v>
-      </c>
-      <c r="B29" t="s">
-        <v>50</v>
       </c>
       <c r="C29">
         <v>70</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>116</v>
+        <v>171</v>
       </c>
       <c r="C30">
         <v>15</v>
@@ -1366,10 +1366,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="C31">
         <v>22</v>
@@ -1377,10 +1377,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>169</v>
       </c>
       <c r="C32">
         <v>10</v>
@@ -1399,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191A2584-3C3A-4478-9F02-7F1AAD4EB254}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,13 +1427,13 @@
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>10</v>
@@ -1441,10 +1441,10 @@
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C2" s="1">
         <v>10</v>
@@ -1454,21 +1454,21 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1">
         <v>6</v>
@@ -1478,13 +1478,13 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1">
         <v>10</v>
@@ -1501,24 +1501,24 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1">
         <v>13</v>
@@ -1527,24 +1527,24 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1">
         <v>9</v>
@@ -1553,24 +1553,24 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="C7" s="1">
         <v>9</v>
@@ -1580,19 +1580,19 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" s="1">
         <v>14</v>
@@ -1601,24 +1601,24 @@
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C9" s="1">
         <v>10</v>
@@ -1628,21 +1628,21 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C10" s="1">
         <v>11</v>
@@ -1652,19 +1652,19 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C11" s="1">
         <v>7</v>
@@ -1674,19 +1674,19 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12" s="1">
         <v>7</v>
@@ -1695,24 +1695,24 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C13" s="1">
         <v>6</v>
@@ -1722,21 +1722,21 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -1746,21 +1746,21 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1">
         <v>7</v>
@@ -1769,24 +1769,24 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C16" s="1">
         <v>7</v>
@@ -1795,24 +1795,24 @@
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C17" s="1">
         <v>17</v>
@@ -1821,24 +1821,24 @@
         <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -1847,24 +1847,24 @@
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C19" s="1">
         <v>11</v>
@@ -1873,24 +1873,24 @@
         <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="C20" s="1">
         <v>9</v>
@@ -1899,24 +1899,24 @@
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="C21" s="1">
         <v>9</v>
@@ -1925,16 +1925,16 @@
         <v>0</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2021,7 +2021,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,74 +2040,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>107</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Prettying up encounter page
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA166F2-B14B-47E1-9306-06629D2B07EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5714679-8507-449A-AD35-1ED96A608A65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="4185" yWindow="3360" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Sample_Custom_Moves" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="227">
   <si>
     <t>Description</t>
   </si>
@@ -696,6 +695,47 @@
   </si>
   <si>
     <t>An airship with a capacity of 13.  Not very good for combat.</t>
+  </si>
+  <si>
+    <t>King Speech</t>
+  </si>
+  <si>
+    <t>+2 to Diplomacy when speaking to rulers of nations</t>
+  </si>
+  <si>
+    <t>Lizard Samurai</t>
+  </si>
+  <si>
+    <t>An lizard creature with a katana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slash: 1d8 damage.  Causes Bleed.
+Bite: 1d10-1 damage. </t>
+  </si>
+  <si>
+    <t>Hammercat</t>
+  </si>
+  <si>
+    <t>A cat wielding a maul</t>
+  </si>
+  <si>
+    <t>Plains, Cave, Mountain, Forest</t>
+  </si>
+  <si>
+    <t>Blinding Bite: 1d4+1 damage.  Causes blind.
+Smash: 1d10+2 damage.</t>
+  </si>
+  <si>
+    <t>Arctic Sniper</t>
+  </si>
+  <si>
+    <t>A white-coated person with a long-range rifle</t>
+  </si>
+  <si>
+    <t>Tundra</t>
+  </si>
+  <si>
+    <t>Shot: 1d10-1 Ice damage.</t>
   </si>
 </sst>
 </file>
@@ -803,8 +843,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BFB740B0-BE3C-48D7-8B7D-8A37A68A10EB}" name="Table1" displayName="Table1" ref="A1:C53" totalsRowShown="0">
   <autoFilter ref="A1:C53" xr:uid="{C8901F27-5F41-43F5-95FC-AD34D4A230AC}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C31">
-    <sortCondition ref="A1:A31"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C42">
+    <sortCondition ref="A1:A53"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{771216C7-D622-489B-9825-DD44002F8F4B}" name="Name"/>
@@ -1148,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD07E7A-4503-4B4C-9531-FC2C793E7E47}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,10 +1223,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>193</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -1194,54 +1234,54 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>159</v>
+        <v>212</v>
+      </c>
+      <c r="B5" t="s">
+        <v>213</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>700</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>160</v>
+        <v>130</v>
+      </c>
+      <c r="B6" t="s">
+        <v>169</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C8">
         <v>15</v>
@@ -1249,87 +1289,87 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
+        <v>110</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>93</v>
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>163</v>
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
       </c>
       <c r="C13">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>165</v>
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="C15">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1337,21 +1377,21 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
+        <v>104</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>164</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C18">
         <v>15</v>
@@ -1359,32 +1399,32 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>54</v>
+        <v>113</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="C19">
-        <v>100</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>168</v>
+        <v>202</v>
+      </c>
+      <c r="B20" t="s">
+        <v>203</v>
       </c>
       <c r="C20">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>6</v>
@@ -1392,65 +1432,65 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>198</v>
       </c>
       <c r="B22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22">
         <v>6</v>
-      </c>
-      <c r="C22">
-        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
+        <v>111</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>200</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>201</v>
       </c>
       <c r="C24">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>175</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>169</v>
+        <v>54</v>
       </c>
       <c r="C26">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C27">
         <v>15</v>
@@ -1458,76 +1498,76 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C28">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>70</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>106</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>171</v>
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
       </c>
       <c r="C30">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>172</v>
+        <v>3</v>
       </c>
       <c r="C31">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>169</v>
+        <v>47</v>
       </c>
       <c r="C32">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="B33" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="B34" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="C34">
         <v>6</v>
@@ -1535,21 +1575,21 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>191</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="C35">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C36">
         <v>6</v>
@@ -1557,68 +1597,68 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>196</v>
-      </c>
-      <c r="B37" t="s">
-        <v>197</v>
+        <v>105</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="C37">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
-        <v>199</v>
+        <v>29</v>
       </c>
       <c r="C38">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="C39">
-        <v>6</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>202</v>
-      </c>
-      <c r="B40" t="s">
-        <v>203</v>
+        <v>106</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="C40">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>204</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="C41">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="B42" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="C42">
-        <v>700</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1634,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191A2584-3C3A-4478-9F02-7F1AAD4EB254}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,142 +1714,142 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>223</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>32</v>
+        <v>224</v>
       </c>
       <c r="C2" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>173</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>137</v>
+        <v>225</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C3" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>173</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>13</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C6" s="1">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C7" s="1">
         <v>9</v>
@@ -1818,24 +1858,24 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>173</v>
+        <v>73</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>177</v>
+        <v>119</v>
       </c>
       <c r="C8" s="1">
         <v>9</v>
@@ -1847,178 +1887,178 @@
         <v>173</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>178</v>
+        <v>139</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>173</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="1">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>14</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
         <v>7</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="1">
-        <v>10</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="C11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>173</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="1">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="1">
-        <v>7</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>173</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="1">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C15" s="1">
         <v>5</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="1">
-        <v>7</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="1">
-        <v>6</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -2027,304 +2067,352 @@
         <v>173</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>185</v>
+        <v>216</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>187</v>
+        <v>217</v>
       </c>
       <c r="C16" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>186</v>
+        <v>221</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>43</v>
+        <v>85</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="C17" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>173</v>
+        <v>38</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C18" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>97</v>
+        <v>185</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>98</v>
+        <v>187</v>
       </c>
       <c r="C19" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="1">
-        <v>17</v>
-      </c>
-      <c r="D20" s="1">
-        <v>3</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D21" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>136</v>
+        <v>38</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C22" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="1">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" s="1">
+        <v>5</v>
+      </c>
+      <c r="D24" s="1">
+        <v>4</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="1">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C26" s="1">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C27" s="1">
         <v>9</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D27" s="1">
         <v>0</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C28" s="1">
         <v>9</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D28" s="1">
         <v>1</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C25" s="1">
-        <v>18</v>
-      </c>
-      <c r="D25" s="1">
-        <v>2</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2339,8 +2427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2F0500-CC62-4BD5-9B1C-FA93D6A66B6C}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,87 +2455,91 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>180</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>153</v>
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>129</v>
+        <v>60</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>129</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>132</v>
+        <v>206</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>158</v>
+        <v>131</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>206</v>
+        <v>124</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>

</xml_diff>

<commit_message>
Change loot drop algo
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5714679-8507-449A-AD35-1ED96A608A65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1DBDE3-43B0-403F-81A8-87975DCF0852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="3360" windowWidth="18000" windowHeight="9360" activeTab="2" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="229">
   <si>
     <t>Description</t>
   </si>
@@ -736,6 +736,12 @@
   </si>
   <si>
     <t>Shot: 1d10-1 Ice damage.</t>
+  </si>
+  <si>
+    <t>Forest Dweller</t>
+  </si>
+  <si>
+    <t>+2 to Sense in a forest</t>
   </si>
 </sst>
 </file>
@@ -2428,7 +2434,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,8 +2548,12 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>

</xml_diff>

<commit_message>
Updating guide + refactoring for better encounter
</commit_message>
<xml_diff>
--- a/site/public/Terra-Machina-Reference-Guide.xlsx
+++ b/site/public/Terra-Machina-Reference-Guide.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\TerraMachina\site\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1DBDE3-43B0-403F-81A8-87975DCF0852}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CC45EB-BE7A-4C8A-A44C-87755A2BDA9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D6459774-64F3-45EA-9086-AC0BDC758EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
     <sheet name="Bestiary" sheetId="2" r:id="rId2"/>
     <sheet name="Sample_Custom_Moves" sheetId="3" r:id="rId3"/>
+    <sheet name="Enemy Data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="240">
   <si>
     <t>Description</t>
   </si>
@@ -742,14 +765,55 @@
   </si>
   <si>
     <t>+2 to Sense in a forest</t>
+  </si>
+  <si>
+    <t>Ground Beetle Armor</t>
+  </si>
+  <si>
+    <t>+1 Armor with Earth attribute</t>
+  </si>
+  <si>
+    <t>Spiderbot</t>
+  </si>
+  <si>
+    <t>A robotic spider with a cannon up top</t>
+  </si>
+  <si>
+    <t>City, Cave</t>
+  </si>
+  <si>
+    <t>Weaknesses</t>
+  </si>
+  <si>
+    <t>Elementals</t>
+  </si>
+  <si>
+    <t>Sky</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Swamp</t>
+  </si>
+  <si>
+    <t>Forest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -777,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -789,6 +853,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,8 +927,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BF78CB2E-8945-46AD-ADE2-A57C11F5C733}" name="Table2" displayName="Table2" ref="A1:H28" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:H28" xr:uid="{D4A8C1E5-52B8-4BF4-8E93-B0DC341A2D32}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BF78CB2E-8945-46AD-ADE2-A57C11F5C733}" name="Table2" displayName="Table2" ref="A1:H34" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:H34" xr:uid="{D4A8C1E5-52B8-4BF4-8E93-B0DC341A2D32}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H28">
     <sortCondition ref="A1:A28"/>
   </sortState>
@@ -1192,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBD07E7A-4503-4B4C-9531-FC2C793E7E47}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,6 +1732,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>229</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C43">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -1678,10 +1754,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191A2584-3C3A-4478-9F02-7F1AAD4EB254}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2420,6 +2496,82 @@
         <v>117</v>
       </c>
     </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -2433,7 +2585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2F0500-CC62-4BD5-9B1C-FA93D6A66B6C}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -2586,4 +2738,244 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A4F592-FADA-4C79-9409-C81769F64DE6}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" cm="1">
+        <f t="array" ref="B2">SUM(LEN(Bestiary!G:G)-LEN(SUBSTITUTE(Bestiary!G:G,A2,"")))/LEN(A2)</f>
+        <v>0</v>
+      </c>
+      <c r="C2" cm="1">
+        <f t="array" ref="C2">SUM(LEN(Bestiary!E:E)-LEN(SUBSTITUTE(Bestiary!E:E,A2,"")))/LEN(A2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" cm="1">
+        <f t="array" ref="B3">SUM(LEN(Bestiary!G:G)-LEN(SUBSTITUTE(Bestiary!G:G,A3,"")))/LEN(A3)</f>
+        <v>3</v>
+      </c>
+      <c r="C3" cm="1">
+        <f t="array" ref="C3">SUM(LEN(Bestiary!E:E)-LEN(SUBSTITUTE(Bestiary!E:E,A3,"")))/LEN(A3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" cm="1">
+        <f t="array" ref="B4">SUM(LEN(Bestiary!G:G)-LEN(SUBSTITUTE(Bestiary!G:G,A4,"")))/LEN(A4)</f>
+        <v>5</v>
+      </c>
+      <c r="C4" cm="1">
+        <f t="array" ref="C4">SUM(LEN(Bestiary!E:E)-LEN(SUBSTITUTE(Bestiary!E:E,A4,"")))/LEN(A4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" cm="1">
+        <f t="array" ref="B5">SUM(LEN(Bestiary!G:G)-LEN(SUBSTITUTE(Bestiary!G:G,A5,"")))/LEN(A5)</f>
+        <v>1</v>
+      </c>
+      <c r="C5" cm="1">
+        <f t="array" ref="C5">SUM(LEN(Bestiary!E:E)-LEN(SUBSTITUTE(Bestiary!E:E,A5,"")))/LEN(A5)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" cm="1">
+        <f t="array" ref="B6">SUM(LEN(Bestiary!G:G)-LEN(SUBSTITUTE(Bestiary!G:G,A6,"")))/LEN(A6)</f>
+        <v>7</v>
+      </c>
+      <c r="C6" cm="1">
+        <f t="array" ref="C6">SUM(LEN(Bestiary!E:E)-LEN(SUBSTITUTE(Bestiary!E:E,A6,"")))/LEN(A6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" cm="1">
+        <f t="array" ref="B7">SUM(LEN(Bestiary!G:G)-LEN(SUBSTITUTE(Bestiary!G:G,A7,"")))/LEN(A7)</f>
+        <v>3</v>
+      </c>
+      <c r="C7" cm="1">
+        <f t="array" ref="C7">SUM(LEN(Bestiary!E:E)-LEN(SUBSTITUTE(Bestiary!E:E,A7,"")))/LEN(A7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" cm="1">
+        <f t="array" ref="B8">SUM(LEN(Bestiary!G:G)-LEN(SUBSTITUTE(Bestiary!G:G,A8,"")))/LEN(A8)</f>
+        <v>4</v>
+      </c>
+      <c r="C8" cm="1">
+        <f t="array" ref="C8">SUM(LEN(Bestiary!E:E)-LEN(SUBSTITUTE(Bestiary!E:E,A8,"")))/LEN(A8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" cm="1">
+        <f t="array" ref="B9">SUM(LEN(Bestiary!G:G)-LEN(SUBSTITUTE(Bestiary!G:G,A9,"")))/LEN(A9)</f>
+        <v>0</v>
+      </c>
+      <c r="C9" cm="1">
+        <f t="array" ref="C9">SUM(LEN(Bestiary!E:E)-LEN(SUBSTITUTE(Bestiary!E:E,A9,"")))/LEN(A9)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" cm="1">
+        <f t="array" ref="B12">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A12,"")))/LEN(A12)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" cm="1">
+        <f t="array" ref="B13">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A13,"")))/LEN(A13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" cm="1">
+        <f t="array" ref="B14">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A14,"")))/LEN(A14)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" cm="1">
+        <f t="array" ref="B15">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A15,"")))/LEN(A15)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>239</v>
+      </c>
+      <c r="B16" cm="1">
+        <f t="array" ref="B16">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A16,"")))/LEN(A16)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" cm="1">
+        <f t="array" ref="B17">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A17,"")))/LEN(A17)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" cm="1">
+        <f t="array" ref="B18">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A18,"")))/LEN(A18)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" cm="1">
+        <f t="array" ref="B19">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A19,"")))/LEN(A19)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" cm="1">
+        <f t="array" ref="B20">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A20,"")))/LEN(A20)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>225</v>
+      </c>
+      <c r="B21" cm="1">
+        <f t="array" ref="B21">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A21,"")))/LEN(A21)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B22" cm="1">
+        <f t="array" ref="B22">SUM(LEN(Bestiary!F:F)-LEN(SUBSTITUTE(Bestiary!F:F,A22,"")))/LEN(A22)</f>
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>